<commit_message>
spreadsheets: Fix bug in project spreadsheet around a ENUM option with a comma
technical_assistance_details, approach
</commit_message>
<xml_diff>
--- a/indigo/spreadsheetform_guides/project_v010.xlsx
+++ b/indigo/spreadsheetform_guides/project_v010.xlsx
@@ -6497,7 +6497,7 @@
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
     </row>
-    <row r="5" customFormat="false" ht="129.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="129.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="12" t="s">
         <v>460</v>
       </c>
@@ -6932,7 +6932,7 @@
     <mergeCell ref="J2:L2"/>
     <mergeCell ref="G3:H3"/>
   </mergeCells>
-  <dataValidations count="6">
+  <dataValidations count="7">
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B5:C33 G5:I33" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
@@ -6945,7 +6945,7 @@
       <formula1>"PUBLIC,PRIVATE,DISPUTED"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E5:E33" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E6:E33" type="list">
       <formula1>"SPO Board Seat (including Observers),Coaching and mentoring,Trainings,Workshops and Boot Camps,Conferences and Other External Events,Access to Networks (External or Peers),Specific Expertise (One-to-One or Groups),Mentoring,Informal Relationship Manageme"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -6955,6 +6955,10 @@
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D5:D33" type="list">
       <formula1>TechAssistDetsCategoryOptions!$A$4:$A$57</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E5" type="list">
+      <formula1>"SPO Board Seat (including Observers),Coaching and mentoring,Trainings and Workshops and Boot Camps,Conferences and Other External Events,Access to Networks (External or Peers),Specific Expertise (One-to-One or Groups),Mentoring,Informal Relationship Manag"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>